<commit_message>
Create code for Zeitstrahl_Analyse.qmd and fix code MCA_Baeume_Szenario0_bis_3
</commit_message>
<xml_diff>
--- a/00_data_raw/Rohdaten_Matrix_Standort_1.xlsx
+++ b/00_data_raw/Rohdaten_Matrix_Standort_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zhaw-my.sharepoint.com/personal/pfeifsar_students_zhaw_ch/Documents/6. Semester MSc UnR/Thesis/R_Project/00_data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{026741F9-F011-448B-B569-C1E045818DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{240DA4B9-D0D9-4A1A-AB34-A88086569571}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{026741F9-F011-448B-B569-C1E045818DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAC28428-BC92-4AA7-8E0F-A5DF12187471}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{03B36E02-7909-4041-A841-6969D6BB26D6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="64">
   <si>
     <t>Konstante</t>
   </si>
@@ -673,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B39B6B9A-559B-46E7-89B7-4D2CB2116C04}">
   <dimension ref="A2:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -946,6 +946,9 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
       <c r="B15" t="s">
         <v>48</v>
       </c>

</xml_diff>